<commit_message>
QA con mi hermana y un amigo
</commit_message>
<xml_diff>
--- a/QA/QA_H-Defense.xlsx
+++ b/QA/QA_H-Defense.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="LbigJ/QhFb7IHNQa4KtU05F+qijyiHZzMFwudE12Tqc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="A34x3ouwxqwiadPkQyux5gNua9R4JwKPYEaIdUPoTMM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
   <si>
     <t>Pruebas con gente externa</t>
   </si>
@@ -39,6 +39,12 @@
     <t>Fácil</t>
   </si>
   <si>
+    <t>Facil</t>
+  </si>
+  <si>
+    <t>Muy facil</t>
+  </si>
+  <si>
     <t>Diseño del HUD</t>
   </si>
   <si>
@@ -51,6 +57,12 @@
     <t>Debería salirte el rango de la torre antes de colorcarla también</t>
   </si>
   <si>
+    <t>no se ve del todo bien el rango deibdo al PopUp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> esta bien lo único que caundo los cañones dañan a los enemigos no les baja la barra de la vida.(dice que al estar uno encima del otro no se aprecia bien la vida de todos)</t>
+  </si>
+  <si>
     <t>Diseño del menú principal</t>
   </si>
   <si>
@@ -60,6 +72,9 @@
     <t>Le hubiese gustado tener un libro de torres como el de enemigos</t>
   </si>
   <si>
+    <t>bien</t>
+  </si>
+  <si>
     <t>Economía del juego</t>
   </si>
   <si>
@@ -75,6 +90,12 @@
     <t>Pensaba que las monedas doradas y las H eran la misma</t>
   </si>
   <si>
+    <t>Muy pocas monedas H en los primeros niveles del juego.</t>
+  </si>
+  <si>
+    <t>lenta</t>
+  </si>
+  <si>
     <t>Estética</t>
   </si>
   <si>
@@ -87,6 +108,12 @@
     <t>Le gustó la música y los sonidos</t>
   </si>
   <si>
+    <t>Buenos en general, falta acabar los sonidos de los efectos cuand oestos acaban</t>
+  </si>
+  <si>
+    <t>Esta guay</t>
+  </si>
+  <si>
     <t>Desbalance del juego</t>
   </si>
   <si>
@@ -99,6 +126,9 @@
     <t>El muro cuesta demasiado y tiene poca vida</t>
   </si>
   <si>
+    <t>El muro no se ha usado practicamente nada junto con la torre de ralentizar</t>
+  </si>
+  <si>
     <t>Manejo de cámara</t>
   </si>
   <si>
@@ -108,6 +138,12 @@
     <t>Le hubiese gustado poder controlar el zoom de la cámara</t>
   </si>
   <si>
+    <t>No se ha dado cuenta de mover la camara con W/A/S/D</t>
+  </si>
+  <si>
+    <t>Movimiento de camara por raton brusco</t>
+  </si>
+  <si>
     <t>Menú de pausa</t>
   </si>
   <si>
@@ -120,6 +156,9 @@
     <t>No lo ha usado mucho</t>
   </si>
   <si>
+    <t>Util para salir al menu principal, poco usado en el Test</t>
+  </si>
+  <si>
     <t>Diseño de mapas</t>
   </si>
   <si>
@@ -132,6 +171,9 @@
     <t>Desincentivar de alguna manera stackear las torres al lado del nexo ya que es demasiado beneficioso. Por ejemplo poner una zona de peligro de vez en cuando o prohibir poner torres una al lado de otra</t>
   </si>
   <si>
+    <t>El tornado hace que al cambiar de rutas algunos enemigos se queden pegando a una torre en lugar de moverse a la nueva ruta</t>
+  </si>
+  <si>
     <t>Propuestas e implementaciones</t>
   </si>
   <si>
@@ -153,9 +195,15 @@
     <t>Poder mover las torres antes de cada oleada</t>
   </si>
   <si>
+    <t>respawns mas rapidos y cerca del núcleo.</t>
+  </si>
+  <si>
     <t>Pruebas de calidad</t>
   </si>
   <si>
+    <t>Verde: Hecho - Rojo: Falta - Azul: Arreglado</t>
+  </si>
+  <si>
     <t>Descripción del error</t>
   </si>
   <si>
@@ -177,7 +225,20 @@
     <t>Funciona el menu de pausa</t>
   </si>
   <si>
-    <t>Tiene el bug de la advertencia, y en los controles no pone nada</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF0000FF"/>
+      </rPr>
+      <t>Tiene el bug de la advertencia</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t>, y en los controles no pone nada</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Ganas monedas doradas matando enemigos </t>
@@ -376,7 +437,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -400,13 +461,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,14 +481,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -462,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -481,6 +553,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -507,7 +585,7 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -518,8 +596,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -790,211 +869,254 @@
       <c r="B5" s="6">
         <v>3.0</v>
       </c>
-    </row>
-    <row r="6" ht="30.0" customHeight="1">
-      <c r="B6" s="6">
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
         <v>3.0</v>
       </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
     </row>
     <row r="7" ht="30.75" customHeight="1">
       <c r="B7" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="30.75" customHeight="1">
+      <c r="B8" s="6">
         <v>3.0</v>
       </c>
     </row>
-    <row r="8" ht="28.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
+    <row r="9" ht="28.5" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
         <v>1.0</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" ht="30.0" customHeight="1">
-      <c r="B9" s="6">
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" ht="30.0" customHeight="1">
+      <c r="B10" s="6">
         <v>2.0</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="6">
-        <v>3.0</v>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="6">
         <v>3.0</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="6">
         <v>2.0</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="B14" s="6">
         <v>3.0</v>
       </c>
-      <c r="C14" s="5" t="s">
+    </row>
+    <row r="15">
+      <c r="B15" s="6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="8">
+    <row r="17">
+      <c r="B17" s="10">
         <v>2.0</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="6">
-        <v>2.0</v>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="6">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="19" ht="42.0" customHeight="1">
+        <v>2.0</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="B19" s="6">
         <v>2.0</v>
       </c>
+      <c r="C19" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="8">
+      <c r="B20" s="6">
         <v>3.0</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="6">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="22" ht="42.0" customHeight="1">
       <c r="B22" s="6">
         <v>2.0</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="6">
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12">
         <v>2.0</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>18</v>
+      <c r="C23" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="6">
+      <c r="B24" s="10">
         <v>3.0</v>
       </c>
+      <c r="C24" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="11">
-        <v>3.0</v>
+      <c r="B25" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="B26" s="6">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" ht="29.25" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="6">
         <v>3.0</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="B29" s="13">
         <v>3.0</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="6">
-        <v>3.0</v>
-      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B30" s="6">
         <v>3.0</v>
       </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="11">
+      <c r="C30" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" ht="29.25" customHeight="1">
+      <c r="B31" s="6">
         <v>3.0</v>
       </c>
+      <c r="C31" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="B32" s="6">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="6">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="6">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -1003,579 +1125,635 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="11">
-        <v>2.0</v>
+      <c r="B36" s="13">
+        <v>3.0</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="B37" s="6">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="B38" s="6">
         <v>2.0</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="B39" s="6">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" ht="31.5" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
       <c r="B40" s="6">
         <v>3.0</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="6">
-        <v>3.0</v>
+      <c r="B41" s="13">
+        <v>2.0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="11">
-        <v>1.0</v>
+      <c r="B42" s="6">
+        <v>2.0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B43" s="6">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="B44" s="6">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" ht="31.5" customHeight="1">
       <c r="B45" s="6">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="12"/>
+      <c r="B46" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="B47" s="6">
         <v>3.0</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" ht="28.5" customHeight="1">
-      <c r="B48" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="B48" s="13">
+        <v>1.0</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>37</v>
+      <c r="A49" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="6">
-        <v>3.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="B52" s="14"/>
+      <c r="C52" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="6">
         <v>3.0</v>
       </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="11">
+      <c r="C53" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" ht="28.5" customHeight="1">
+      <c r="B54" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="B55" s="10">
         <v>2.0</v>
       </c>
-    </row>
-    <row r="53" ht="28.5" customHeight="1">
-      <c r="A53" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="5" t="s">
-        <v>41</v>
+      <c r="C55" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
+      <c r="B56" s="6">
+        <v>3.0</v>
+      </c>
       <c r="C56" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="5" t="s">
-        <v>43</v>
+      <c r="B57" s="6">
+        <v>3.0</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="27.0" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" ht="27.0" customHeight="1">
-      <c r="A67" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B68" s="19"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="19"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B70" s="20"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="17" t="s">
+      <c r="B58" s="13">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="59" ht="28.5" customHeight="1">
+      <c r="A59" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="5" t="s">
+      <c r="B59" s="16"/>
+      <c r="C59" s="9" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="C60" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="C61" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="C62" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="C63" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="C64" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="27.0" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" s="20"/>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B73" s="21"/>
+      <c r="A72" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" ht="27.0" customHeight="1">
+      <c r="A73" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="20"/>
       <c r="C73" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="20"/>
+      <c r="A74" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" s="21"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="20"/>
+      <c r="A75" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="21"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B76" s="20"/>
+      <c r="A76" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="22"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B77" s="22"/>
+      <c r="A77" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="23"/>
+      <c r="C77" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="20"/>
+      <c r="A78" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="22"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B79" s="20"/>
+      <c r="A79" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="24"/>
+      <c r="C79" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B80" s="20"/>
+      <c r="A80" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="22"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B81" s="20"/>
+      <c r="A81" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" s="22"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B82" s="20"/>
+      <c r="A82" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" s="22"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B83" s="20"/>
+      <c r="A83" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B83" s="25"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B84" s="20"/>
+      <c r="A84" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="22"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B85" s="20"/>
+      <c r="A85" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B85" s="22"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B86" s="21"/>
-      <c r="C86" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="A86" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="22"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B87" s="21"/>
-      <c r="C87" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="A87" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="22"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B88" s="20"/>
+      <c r="A88" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" s="22"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89" s="20"/>
+      <c r="A89" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" s="22"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B90" s="20"/>
+      <c r="A90" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90" s="22"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B91" s="21"/>
-      <c r="C91" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="A91" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="22"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B92" s="20"/>
+      <c r="A92" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="23"/>
+      <c r="C92" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="25"/>
+      <c r="A93" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="23"/>
+      <c r="C93" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" s="20"/>
+      <c r="A94" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B94" s="22"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B95" s="20"/>
+      <c r="A95" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" s="22"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B96" s="25"/>
+      <c r="A96" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="22"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B97" s="20"/>
+      <c r="A97" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="24"/>
+      <c r="C97" s="9" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B98" s="20"/>
+      <c r="A98" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B98" s="22"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B99" s="25"/>
+      <c r="A99" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B99" s="28"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B100" s="25"/>
+      <c r="A100" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="22"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B101" s="25"/>
+      <c r="A101" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" s="22"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="25"/>
+      <c r="A102" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" s="28"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="20"/>
+      <c r="A103" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" s="22"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B104" s="20"/>
+      <c r="A104" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="22"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B105" s="25"/>
+      <c r="A105" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="28"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="A106" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" s="28"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B107" s="25"/>
+      <c r="A107" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B107" s="28"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B108" s="25"/>
+      <c r="A108" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B108" s="28"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B109" s="25"/>
+      <c r="A109" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B109" s="22"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B110" s="20"/>
+      <c r="A110" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B110" s="22"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B111" s="21"/>
-      <c r="C111" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="A111" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B111" s="28"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B112" s="20"/>
+      <c r="A112" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B112" s="24"/>
+      <c r="C112" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B113" s="20"/>
+      <c r="A113" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B113" s="28"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B114" s="20"/>
+      <c r="A114" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" s="28"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B115" s="25"/>
+      <c r="A115" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115" s="28"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B116" s="25"/>
+      <c r="A116" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B116" s="22"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B117" s="25"/>
+      <c r="A117" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B117" s="24"/>
+      <c r="C117" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B118" s="20"/>
+      <c r="A118" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B118" s="22"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B119" s="20"/>
+      <c r="A119" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B119" s="22"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B120" s="20"/>
+      <c r="A120" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" s="22"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B121" s="20"/>
+      <c r="A121" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B121" s="28"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B122" s="20"/>
+      <c r="A122" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B122" s="28"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B123" s="20"/>
+      <c r="A123" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B123" s="28"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B124" s="20"/>
+      <c r="A124" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B124" s="22"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B125" s="21"/>
-      <c r="C125" s="5" t="s">
-        <v>114</v>
-      </c>
+      <c r="A125" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B125" s="22"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B126" s="20"/>
+      <c r="A126" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B126" s="22"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B127" s="21"/>
-      <c r="C127" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
+      <c r="A127" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B127" s="22"/>
+    </row>
+    <row r="128" ht="15.75" customHeight="1">
+      <c r="A128" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B128" s="22"/>
+    </row>
+    <row r="129" ht="15.75" customHeight="1">
+      <c r="A129" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B129" s="22"/>
+    </row>
+    <row r="130" ht="15.75" customHeight="1">
+      <c r="A130" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B130" s="22"/>
+    </row>
+    <row r="131" ht="15.75" customHeight="1">
+      <c r="A131" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B131" s="24"/>
+      <c r="C131" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" ht="15.75" customHeight="1">
+      <c r="A132" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132" s="22"/>
+    </row>
+    <row r="133" ht="15.75" customHeight="1">
+      <c r="A133" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133" s="23"/>
+      <c r="C133" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="134" ht="15.75" customHeight="1"/>
     <row r="135" ht="15.75" customHeight="1"/>
     <row r="136" ht="15.75" customHeight="1"/>
@@ -2443,6 +2621,12 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>